<commit_message>
Remove check already, some comments, doxygen scripts
</commit_message>
<xml_diff>
--- a/doc/algo.xlsx
+++ b/doc/algo.xlsx
@@ -135,6 +135,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -144,6 +145,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -152,6 +154,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">N+1</t>
     </r>
@@ -161,6 +164,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -174,6 +178,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -183,6 +188,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -191,6 +197,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">M-1</t>
     </r>
@@ -200,6 +207,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -259,6 +267,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -280,6 +289,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -453,10 +463,10 @@
       <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="15.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="31.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="29.03"/>

</xml_diff>